<commit_message>
dsa graphs, web css
</commit_message>
<xml_diff>
--- a/java/LC_Graphs.xlsx
+++ b/java/LC_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFF7649D-2812-46AD-ACD2-C2C01EC21480}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036A3B34-A415-4CCE-8871-BE9F25E34F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
   <si>
     <t>Question</t>
   </si>
@@ -55,6 +55,15 @@
   </si>
   <si>
     <t>The crux is Cycle check DFS. Basically we do a for loop on the adj list, and do a dfs at each node using graph coloring, where colors (int) represent states. 0: not visited, 1: safe, 2: unsafe. We then do DFS to check for cycles. Enum makes it more clear and is good practice.</t>
+  </si>
+  <si>
+    <t>1129.Shortest Path with Alternating Colors</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/shortest-path-with-alternating-colors/solutions/339964/java-python-bfs/?envType=study-plan-v2&amp;envId=graph-theory </t>
+  </si>
+  <si>
+    <t>Graph BFS but with alternating colors and color tracking.</t>
   </si>
 </sst>
 </file>
@@ -399,17 +408,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="39.28515625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="17.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="115.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="81.85546875" customWidth="1"/>
     <col min="5" max="5" width="160.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -447,9 +456,27 @@
         <v>8</v>
       </c>
     </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{500ED57E-6BC3-4E42-9C00-8C2028A5E9AC}"/>
+    <hyperlink ref="E3" r:id="rId2" xr:uid="{F414B125-C3DA-4E86-BBAE-7E3C3182242A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa graphs, sql, python
</commit_message>
<xml_diff>
--- a/java/LC_Graphs.xlsx
+++ b/java/LC_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{036A3B34-A415-4CCE-8871-BE9F25E34F0B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0676413F-E45F-4B22-8D52-DB95AD330358}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Question</t>
   </si>
@@ -64,6 +64,18 @@
   </si>
   <si>
     <t>Graph BFS but with alternating colors and color tracking.</t>
+  </si>
+  <si>
+    <t>934. Shortest Bridge</t>
+  </si>
+  <si>
+    <t>BFS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/shortest-bridge/solutions/1448914/java-easy-approach-with-explanation-bfs-dfs-preorder-graph/?envType=study-plan-v2&amp;envId=graph-theory </t>
+  </si>
+  <si>
+    <t>Use DFS to find one island cell and traverse the entire island to add to the queue and mark as visited, then use bfs to find the nearest other island cell.</t>
   </si>
 </sst>
 </file>
@@ -408,10 +420,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,10 +485,28 @@
         <v>11</v>
       </c>
     </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>15</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{500ED57E-6BC3-4E42-9C00-8C2028A5E9AC}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{F414B125-C3DA-4E86-BBAE-7E3C3182242A}"/>
+    <hyperlink ref="E4" r:id="rId3" xr:uid="{4DACCFB1-20E1-4A67-B308-3F2F39440BF5}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa graphs and sql
</commit_message>
<xml_diff>
--- a/java/LC_Graphs.xlsx
+++ b/java/LC_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E74A8DB8-C65C-4BA9-8FF4-9700B3D9E1F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D7BFDE6-E0E4-4951-A433-0066D54AF643}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="25">
   <si>
     <t>Question</t>
   </si>
@@ -91,6 +91,15 @@
   </si>
   <si>
     <t>Decrement the indegree count, or "trust" of the outgoing person (person[0]) and increment indegree count of the receiving vertex (person[1]). At the end, find the person with the indegree count of n - 1.</t>
+  </si>
+  <si>
+    <t>1557. Minimum Number of Vertices to Reach All Nodes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/minimum-number-of-vertices-to-reach-all-nodes/solutions/805685/java-c-python-nodes-with-no-in-degree/?envType=study-plan-v2&amp;envId=graph-theory </t>
+  </si>
+  <si>
+    <t>Basically find all the nodes with in-degree = 0. Because you can't get to these nodes from anywhere, and once you have all of these you can visit the next level of nodes, and so on. We don't need to do graph traversal, but just look at the vertices with a seen[] map.</t>
   </si>
 </sst>
 </file>
@@ -442,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,12 +550,30 @@
         <v>20</v>
       </c>
     </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" t="s">
+        <v>24</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{500ED57E-6BC3-4E42-9C00-8C2028A5E9AC}"/>
     <hyperlink ref="E3" r:id="rId2" xr:uid="{F414B125-C3DA-4E86-BBAE-7E3C3182242A}"/>
     <hyperlink ref="E4" r:id="rId3" xr:uid="{4DACCFB1-20E1-4A67-B308-3F2F39440BF5}"/>
     <hyperlink ref="E5" r:id="rId4" xr:uid="{F89768BD-B7BC-4F9D-9F7E-392F4D206FD1}"/>
+    <hyperlink ref="E6" r:id="rId5" xr:uid="{2B4D03C4-07A6-4BF3-855F-A54D26ED446F}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
dsa graphs, sql, js
</commit_message>
<xml_diff>
--- a/java/LC_Graphs.xlsx
+++ b/java/LC_Graphs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JP\Desktop\Home_folder\workspace\library\java\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8E628E66-D20A-45CD-817D-EEA33277AE54}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52C7A0A4-540D-4133-8BEC-FC68FF097026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="35">
   <si>
     <t>Question</t>
   </si>
@@ -118,6 +118,18 @@
   </si>
   <si>
     <t xml:space="preserve">https://leetcode.com/problems/is-graph-bipartite/solutions/115487/java-clean-dfs-solution-with-explanation/?envType=study-plan-v2&amp;envId=graph-theory </t>
+  </si>
+  <si>
+    <t>721. Accounts Merge</t>
+  </si>
+  <si>
+    <t>Union Find</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://leetcode.com/problems/accounts-merge/solutions/1601980/java-solution-using-unionfind-beats-99-87-of-submissions/?envType=study-plan-v2&amp;envId=graph-theory </t>
+  </si>
+  <si>
+    <t>Union Find, use hash for unique emails, and a hash for unique accounts, then collect the emails from the accounts hash and add account name at index 0 for the result list.</t>
   </si>
 </sst>
 </file>
@@ -469,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -619,6 +631,23 @@
         <v>30</v>
       </c>
     </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>31</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>32</v>
+      </c>
+      <c r="D9" t="s">
+        <v>34</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>33</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{500ED57E-6BC3-4E42-9C00-8C2028A5E9AC}"/>
@@ -628,6 +657,7 @@
     <hyperlink ref="E6" r:id="rId5" xr:uid="{2B4D03C4-07A6-4BF3-855F-A54D26ED446F}"/>
     <hyperlink ref="E7" r:id="rId6" xr:uid="{19351CDE-4859-439A-9E78-66082EA3F81E}"/>
     <hyperlink ref="E8" r:id="rId7" xr:uid="{BBEEC08C-F0B6-4C29-A5A7-8A264F4DEAF1}"/>
+    <hyperlink ref="E9" r:id="rId8" xr:uid="{C882C2E8-4DC1-43C8-A775-AFA1A09094A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>